<commit_message>
Add ADCS log telemetry (WOD) frame and payload
A couple minor edits to rag and wod telemetry
</commit_message>
<xml_diff>
--- a/genSpacecraft/DownlinkSpecGolf-T.xlsx
+++ b/genSpacecraft/DownlinkSpecGolf-T.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2374" uniqueCount="713">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2434" uniqueCount="720">
   <si>
     <t xml:space="preserve">//</t>
   </si>
@@ -2142,6 +2142,27 @@
   </si>
   <si>
     <t xml:space="preserve">pad420</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Structure:ADCSLogData_t, file:ADCSLogDataDownlink.h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Structure:ADCSLog_t, file:ADCSLogDownlink.h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LogType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADCS Log Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADCSLog</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LogFrameNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Log Frame Number</t>
   </si>
   <si>
     <t xml:space="preserve">Payloads per Frame</t>
@@ -2527,10 +2548,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Q425"/>
+  <dimension ref="A1:Q1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A215" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I226" activeCellId="0" sqref="I226"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A417" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H431" activeCellId="0" sqref="H431:H432"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2538,14 +2559,16 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16.24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="53.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="3" width="31.22"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="8.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="14.74"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="22.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="10.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="67.33"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="8" style="3" width="8.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="13.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="4" width="8.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="11" style="5" width="8.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="5" width="11.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="5" width="12.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="5" width="6.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="18.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="3" width="8.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="13.22"/>
@@ -21256,12 +21279,351 @@
         <v>36</v>
       </c>
     </row>
-    <row r="425" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C425" s="3"/>
-      <c r="H425" s="3"/>
-      <c r="J425" s="47"/>
-      <c r="O425" s="3"/>
-    </row>
+    <row r="425" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A425" s="41" t="s">
+        <v>707</v>
+      </c>
+      <c r="B425" s="12"/>
+      <c r="C425" s="40"/>
+      <c r="D425" s="13"/>
+      <c r="E425" s="13"/>
+      <c r="F425" s="13"/>
+      <c r="G425" s="13"/>
+      <c r="H425" s="13"/>
+      <c r="I425" s="14"/>
+    </row>
+    <row r="426" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A426" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B426" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C426" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D426" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="E426" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="F426" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="G426" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="H426" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="I426" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="J426" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="K426" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="L426" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="M426" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="N426" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="O426" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="P426" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q426" s="15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="427" customFormat="false" ht="50.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B427" s="30" t="s">
+        <v>448</v>
+      </c>
+      <c r="C427" s="22" t="s">
+        <v>449</v>
+      </c>
+      <c r="D427" s="22" t="n">
+        <v>5168</v>
+      </c>
+      <c r="E427" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="F427" s="22" t="s">
+        <v>120</v>
+      </c>
+      <c r="G427" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="H427" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="I427" s="23" t="s">
+        <v>450</v>
+      </c>
+      <c r="J427" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="K427" s="27" t="n">
+        <f aca="false">J427/8</f>
+        <v>0</v>
+      </c>
+      <c r="L427" s="27" t="n">
+        <f aca="false">J427/16</f>
+        <v>0</v>
+      </c>
+      <c r="M427" s="27" t="n">
+        <f aca="false">J427/32</f>
+        <v>0</v>
+      </c>
+      <c r="N427" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="O427" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="P427" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q427" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="428" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A428" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B428" s="25"/>
+      <c r="I428" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="J428" s="4" t="n">
+        <f aca="false">J427+D427</f>
+        <v>5168</v>
+      </c>
+      <c r="K428" s="27" t="n">
+        <f aca="false">J428/8</f>
+        <v>646</v>
+      </c>
+      <c r="L428" s="27" t="n">
+        <f aca="false">J428/16</f>
+        <v>323</v>
+      </c>
+      <c r="M428" s="27" t="n">
+        <f aca="false">J428/32</f>
+        <v>161.5</v>
+      </c>
+    </row>
+    <row r="429" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A429" s="41" t="s">
+        <v>708</v>
+      </c>
+      <c r="B429" s="12"/>
+      <c r="C429" s="40"/>
+      <c r="D429" s="13"/>
+      <c r="E429" s="13"/>
+      <c r="F429" s="13"/>
+      <c r="G429" s="13"/>
+      <c r="H429" s="13"/>
+      <c r="I429" s="14"/>
+    </row>
+    <row r="430" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A430" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B430" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C430" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D430" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="E430" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="F430" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="G430" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="H430" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="I430" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="J430" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="K430" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="L430" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="M430" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="N430" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="O430" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="P430" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q430" s="15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="431" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B431" s="30" t="s">
+        <v>709</v>
+      </c>
+      <c r="C431" s="30" t="s">
+        <v>439</v>
+      </c>
+      <c r="D431" s="26" t="n">
+        <v>16</v>
+      </c>
+      <c r="E431" s="37" t="s">
+        <v>26</v>
+      </c>
+      <c r="F431" s="23" t="s">
+        <v>461</v>
+      </c>
+      <c r="G431" s="37" t="n">
+        <v>1</v>
+      </c>
+      <c r="H431" s="38" t="s">
+        <v>27</v>
+      </c>
+      <c r="I431" s="27" t="s">
+        <v>710</v>
+      </c>
+      <c r="J431" s="4" t="n">
+        <f aca="false">J428</f>
+        <v>5168</v>
+      </c>
+      <c r="K431" s="27" t="n">
+        <f aca="false">J431/8</f>
+        <v>646</v>
+      </c>
+      <c r="L431" s="27" t="n">
+        <f aca="false">J431/16</f>
+        <v>323</v>
+      </c>
+      <c r="M431" s="27" t="n">
+        <f aca="false">J431/32</f>
+        <v>161.5</v>
+      </c>
+      <c r="N431" s="1" t="s">
+        <v>711</v>
+      </c>
+      <c r="O431" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="P431" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q431" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="432" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B432" s="30" t="s">
+        <v>712</v>
+      </c>
+      <c r="C432" s="30" t="s">
+        <v>435</v>
+      </c>
+      <c r="D432" s="26" t="n">
+        <v>32</v>
+      </c>
+      <c r="E432" s="37" t="s">
+        <v>26</v>
+      </c>
+      <c r="F432" s="23"/>
+      <c r="G432" s="23" t="n">
+        <v>1</v>
+      </c>
+      <c r="H432" s="38" t="s">
+        <v>27</v>
+      </c>
+      <c r="I432" s="27" t="s">
+        <v>713</v>
+      </c>
+      <c r="J432" s="4" t="n">
+        <f aca="false">J431+D431</f>
+        <v>5184</v>
+      </c>
+      <c r="K432" s="27" t="n">
+        <f aca="false">J432/8</f>
+        <v>648</v>
+      </c>
+      <c r="L432" s="27" t="n">
+        <f aca="false">J432/16</f>
+        <v>324</v>
+      </c>
+      <c r="M432" s="27" t="n">
+        <f aca="false">J432/32</f>
+        <v>162</v>
+      </c>
+      <c r="N432" s="1" t="s">
+        <v>711</v>
+      </c>
+      <c r="O432" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="P432" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q432" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="433" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A433" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B433" s="25"/>
+      <c r="I433" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="J433" s="4" t="n">
+        <f aca="false">J432+D432</f>
+        <v>5216</v>
+      </c>
+      <c r="K433" s="27" t="n">
+        <f aca="false">J433/8</f>
+        <v>652</v>
+      </c>
+      <c r="L433" s="27" t="n">
+        <f aca="false">J433/16</f>
+        <v>326</v>
+      </c>
+      <c r="M433" s="27" t="n">
+        <f aca="false">J433/32</f>
+        <v>163</v>
+      </c>
+    </row>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="B1:I1"/>
@@ -21276,10 +21638,12 @@
     <hyperlink ref="A230" r:id="rId2" display="Structure:radWodSpecific_t, file:radWodSpecificDownlink.h"/>
     <hyperlink ref="A245" r:id="rId3" display="Structure:infrequentDownlink_t,file:infrequentDownlink.h"/>
     <hyperlink ref="A309" r:id="rId4" display="Structure:rt1Errors_t,file:rt1ErrorsDownlink.h"/>
+    <hyperlink ref="A425" r:id="rId5" display="Structure:ADCSLogData_t, file:ADCSLogDataDownlink.h"/>
+    <hyperlink ref="A429" r:id="rId6" display="Structure:ADCSLog_t, file:ADCSLogDownlink.h"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -21295,10 +21659,10 @@
   <dimension ref="B6:I20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F8" activeCellId="0" sqref="F8"/>
+      <selection pane="topLeft" activeCell="F8" activeCellId="1" sqref="H431:H432 F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1484375" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.11"/>
@@ -21308,22 +21672,22 @@
     <row r="6" s="48" customFormat="true" ht="34.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B6" s="49"/>
       <c r="C6" s="49" t="s">
-        <v>707</v>
+        <v>714</v>
       </c>
       <c r="D6" s="49" t="s">
-        <v>708</v>
+        <v>715</v>
       </c>
       <c r="E6" s="49" t="s">
-        <v>709</v>
+        <v>716</v>
       </c>
       <c r="F6" s="49" t="s">
-        <v>710</v>
+        <v>717</v>
       </c>
       <c r="G6" s="49" t="s">
-        <v>711</v>
+        <v>718</v>
       </c>
       <c r="H6" s="49" t="s">
-        <v>712</v>
+        <v>719</v>
       </c>
       <c r="I6" s="49"/>
     </row>
@@ -21694,7 +22058,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>